<commit_message>
Code Review 1 update
</commit_message>
<xml_diff>
--- a/Docs/Group E Individual team members contribution.xlsx
+++ b/Docs/Group E Individual team members contribution.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/98dbd5f269b99770/Desktop/Software Engineering Methods/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B2A1FB7-D6A3-4539-AD28-468FA4843930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{2B2A1FB7-D6A3-4539-AD28-468FA4843930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A28BB6BA-7C1D-4306-9D4A-1DF978FE18E0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="23280" windowHeight="12600" xr2:uid="{F1E11C5F-57A9-4A99-A8DF-9B4B512AB1B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F1E11C5F-57A9-4A99-A8DF-9B4B512AB1B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -439,17 +439,19 @@
   <dimension ref="A2:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="14.109375" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="16.109375" hidden="1" customWidth="1"/>
+    <col min="6" max="6" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -466,11 +468,13 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>40646470</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1">
+        <v>25</v>
+      </c>
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -478,11 +482,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>40679395</v>
       </c>
-      <c r="B4" s="1"/>
+      <c r="B4" s="1">
+        <v>25</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -490,11 +496,13 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>40674826</v>
       </c>
-      <c r="B5" s="1"/>
+      <c r="B5" s="1">
+        <v>25</v>
+      </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
@@ -502,11 +510,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>40582347</v>
       </c>
-      <c r="B6" s="1"/>
+      <c r="B6" s="1">
+        <v>25</v>
+      </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
@@ -514,7 +524,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>5</v>
       </c>

</xml_diff>